<commit_message>
changed build number to 5200
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A224C5-0B46-4587-A51C-AAB69EC90DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4FE251-A7B4-431D-B290-ED2F28F87576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated to build 6572
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C196F443-1F2D-4038-A0D5-CBF1C50F2907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65007ED-2472-4F69-9555-D67A6A5D9861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="7">
-        <v>5640</v>
+        <v>6572</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
spherical fog is back for 1.21.6
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DA6F05-EF65-4106-A0BA-A5F762BB55EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FB345B-26BF-453C-A207-A64CF6CC6705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Added trim template item textures</t>
+  </si>
+  <si>
+    <t>spherical fog is back for 1.21.6</t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -676,6 +679,11 @@
         <v>22</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated build to 7318
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE72FFA9-3612-4CDF-845A-6776D3966699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA34CAE0-A543-4CF7-B2CB-D4B33D688D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="7">
-        <v>7144</v>
+        <v>7318</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7707
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D932F5-A237-4EDE-9E89-9E0850E6B4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B1BCB9-80E2-4482-9829-93798A547E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7578</v>
+        <v>7707</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated to build 7792
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B1BCB9-80E2-4482-9829-93798A547E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B2869A-3541-41A6-96A1-6631FBCC5AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7707</v>
+        <v>7792</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
updated build to 7814
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD09CFA-EB07-48FD-8E7E-8B35B29874A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F14308E-3877-4F1F-AED1-11F3389C5D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -65,7 +65,7 @@
     <t>10.0.6</t>
   </si>
   <si>
-    <t>Improved fog shaders for 1.21.6</t>
+    <t>Improved fog shaders for 1.21.2+</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7792</v>
+        <v>7814</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7817
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F14308E-3877-4F1F-AED1-11F3389C5D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF7F16-FBA1-48E5-BA2F-6EB9DB818BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7814</v>
+        <v>7817</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7821
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF7F16-FBA1-48E5-BA2F-6EB9DB818BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA6F3CA-F8E9-48D3-BB1C-CCC1C330D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Improved fog shaders for 1.21.2+</t>
+  </si>
+  <si>
+    <t>Changed lightmap 1.21.6+ (Vanilla)</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -551,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7817</v>
+        <v>7821</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
@@ -572,6 +575,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to build 7829
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic_Reimagined_LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA6F3CA-F8E9-48D3-BB1C-CCC1C330D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF177A-D6A6-43BA-A702-339522C93C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7821</v>
+        <v>7829</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7830
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic_Reimagined_LTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF177A-D6A6-43BA-A702-339522C93C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4774F506-36B7-4C60-8335-ADE5E24F5FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7829</v>
+        <v>7830</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7840
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4774F506-36B7-4C60-8335-ADE5E24F5FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE52584F-49F9-4019-BFCC-184807124C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -68,7 +68,7 @@
     <t>Improved fog shaders for 1.21.2+</t>
   </si>
   <si>
-    <t>Changed lightmap 1.21.6+ (Vanilla)</t>
+    <t>Changed lightmap 1.21+ (Vanilla)</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7830</v>
+        <v>7840</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
updated build to 7842
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE52584F-49F9-4019-BFCC-184807124C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA36F3D2-1AD9-494E-B3CA-0568066BBFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7840</v>
+        <v>7842</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Fixed mipmaps not working
- Purged textures
- Updated Core version to 7853
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA36F3D2-1AD9-494E-B3CA-0568066BBFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0372475-0CCE-4FC9-88D1-2F9AD4F01FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Changed lightmap 1.21+ (Vanilla)</t>
+  </si>
+  <si>
+    <t>Fixed mipmaps not working</t>
+  </si>
+  <si>
+    <t>Fixed cloud shaders</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -554,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7842</v>
+        <v>7853</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
@@ -580,6 +586,16 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated to build 7854
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0372475-0CCE-4FC9-88D1-2F9AD4F01FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C9C59B-3A22-4C81-86D3-1B7CF60C6CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -560,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7853</v>
+        <v>7854</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
updated to build 7858
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C9C59B-3A22-4C81-86D3-1B7CF60C6CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6D9334-C9EA-4502-9FAD-3148C96BE6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -560,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7854</v>
+        <v>7858</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated to build 7880
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD77B35-B02E-460F-8A11-B9E35D2A0A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584AF38A-76AF-4C6C-8309-7D52F86C71A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7">
-        <v>7868</v>
+        <v>7880</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated to build 7883
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EAC6CA-5B35-4675-AEF8-E85BA646D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A0413-A768-4DBE-AAF5-BF853DF7BF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7">
-        <v>7880</v>
+        <v>7883</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Update changelog.xlsx to reflect recent changes
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90852480-D9EC-443E-A06D-E76F34773B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC16948-F653-4D6D-B59D-A2A453F5CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Changed Vex CEM</t>
+  </si>
+  <si>
+    <t>Fixed Rabbit CEM</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -612,6 +615,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to build 7931
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D0DB17-67FE-4927-BB12-5285CB352794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21873DB-8E68-48B3-9B20-E2C8C15EAB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7">
-        <v>7929</v>
+        <v>7931</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated build to 7950
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21873DB-8E68-48B3-9B20-E2C8C15EAB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C04C3E1-3CC5-4555-A5D4-FA5BDCB01F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Refactor bat model and update texture for improved visuals</t>
+  </si>
+  <si>
+    <t>Added support for Polytone</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -628,6 +631,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
improved fog.glsl shader for 1.21.2
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9EA202-5E79-4F87-8925-DE4427068182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3677198-2BC5-4319-99D3-340FB37B9B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>VulkanMod compatibility</t>
+  </si>
+  <si>
+    <t>Removed OptiFine Lightmaps</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -636,6 +639,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
moved lightmap for older versions of Classic Reimagined
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3677198-2BC5-4319-99D3-340FB37B9B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8102102C-A510-48A2-9E76-D774E8F9DB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Removed OptiFine Lightmaps</t>
+  </si>
+  <si>
+    <t>Reimproved lighting (Vanilla, OptiFine)</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -644,6 +647,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to build 7972
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8102102C-A510-48A2-9E76-D774E8F9DB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32327A40-3C46-47C2-B8E6-9728456DF7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="7">
-        <v>7950</v>
+        <v>7972</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">

</xml_diff>

<commit_message>
Updated to build 7977
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93687F-0B60-47D7-B11E-5D2EE75A9763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7672B-0E7E-46CB-A38D-81D9D341861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -556,7 +556,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="7">
-        <v>7972</v>
+        <v>7977</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
@@ -618,62 +618,62 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update particle textures and changelog
- Updated sweep_6.png and sweep_7.png particle textures.
- Modified changelog.xlsx to reflect recent changes.
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\better_default\resourcepacks\Classic Reimagined LTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F979A9D-783D-450C-8DBE-4A9892D5B51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AED3B8-71A6-4B13-9D5F-D12FF87C8439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78FFC81C-E409-4A91-B2FB-77FB25E4AB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -65,7 +65,13 @@
     <t>VulkanMod compatibility</t>
   </si>
   <si>
-    <t>Fixed enchantment glint not working</t>
+    <t>Changed panorama</t>
+  </si>
+  <si>
+    <t>Fixed enchantment glint not working (1.21.2)</t>
+  </si>
+  <si>
+    <t>Fixed VRAM leakage</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE7BC97-825F-4E4F-95C0-CEEB2FCB8921}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -569,7 +575,17 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor BETA_LIGHT array for improved readability in lightmap.fsh
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hexy\AppData\Roaming\ModrinthApp\profiles\Classic Reimagined 10 Dependency Modpack\resourcepacks\Classic Reimagined LTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hexy\AppData\Roaming\ModrinthApp\profiles\Classic Reimagined 10 Dependency Modpack\resourcepacks\Classic Reimagined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB0BEE-58AE-4500-8B51-EAD379F39A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F941A660-FDF3-4B82-B24B-496A95DBF438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Known issues/Goals</t>
   </si>
   <si>
-    <t>1.21.6</t>
-  </si>
-  <si>
-    <t>10.0.7</t>
-  </si>
-  <si>
     <t>VulkanMod compatibility</t>
   </si>
   <si>
@@ -73,6 +67,18 @@
   </si>
   <si>
     <t>Fixed fire model (Sodium)</t>
+  </si>
+  <si>
+    <t>Changed dried ghast textures</t>
+  </si>
+  <si>
+    <t>10.0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Released Classic Reimagined 11 (WIP) </t>
+  </si>
+  <si>
+    <t>1.21.7</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -482,22 +488,22 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7">
-        <v>8200</v>
+        <v>8255</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
@@ -506,37 +512,47 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GLSL version in shaders to 460
Upgraded GLSL version from 150 to 460 in lightmap and cloud shaders for 1.21.2. Minor formatting adjustment in terrain.vsh for 1.21.6. Updated changelog.xlsx to reflect these changes.
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hexy\AppData\Roaming\ModrinthApp\profiles\Classic Reimagined 10 Dependency Modpack\resourcepacks\Classic Reimagined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Classic Reimagined 10\resourcepacks\Classic-Reimagined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F941A660-FDF3-4B82-B24B-496A95DBF438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB895662-07E5-452C-A9DA-F63FE4CB23C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>1.21.7</t>
+  </si>
+  <si>
+    <t>Fixed soul fire model (Sodium)</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -555,6 +558,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:B3"/>

</xml_diff>

<commit_message>
updated to the 25w31a snapshot
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Classic Reimagined 10\resourcepacks\Classic-Reimagined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB895662-07E5-452C-A9DA-F63FE4CB23C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405BCF2-F3AB-452E-9A2B-7B5DF87D0F80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -78,17 +78,20 @@
     <t xml:space="preserve">Released Classic Reimagined 11 (WIP) </t>
   </si>
   <si>
-    <t>1.21.7</t>
-  </si>
-  <si>
     <t>Fixed soul fire model (Sodium)</t>
+  </si>
+  <si>
+    <t>Added support for 1.21.9</t>
+  </si>
+  <si>
+    <t>1.21.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,19 +463,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="5" width="18.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="5" width="18.25" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,22 +492,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="7">
-        <v>8255</v>
+        <v>9650</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -513,53 +516,58 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed copper lantern textures
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PrismLauncher\instances\1.21.7\minecraft\resourcepacks\Classic-Reimagined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595A1F54-9B4D-475C-A538-19D679EA1ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D65A67A-8062-483D-B12D-07927FF61C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Known issues (Compatibility)</t>
+  </si>
+  <si>
+    <t>Changed copper lantern textures</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -617,6 +620,11 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>